<commit_message>
Student & Hall Modified
</commit_message>
<xml_diff>
--- a/Student Details DMS Final.xlsx
+++ b/Student Details DMS Final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\dms_msc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE775705-BF8B-49B6-ABAF-41C0DC1BFCD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B46DC07-5545-4F0B-AAB9-E2F748B91E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>S.N</t>
   </si>
@@ -49,13 +49,19 @@
   </si>
   <si>
     <t>S. M. Parvez Jewel</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,14 @@
     <font>
       <b/>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,12 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,12 +414,12 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -414,8 +429,11 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -425,8 +443,11 @@
       <c r="C5">
         <v>41134</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -436,8 +457,11 @@
       <c r="C6">
         <v>41144</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -447,8 +471,11 @@
       <c r="C7">
         <v>41148</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -457,6 +484,9 @@
       </c>
       <c r="C8">
         <v>41428</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Student with Hall Info Add
</commit_message>
<xml_diff>
--- a/Student Details DMS Final.xlsx
+++ b/Student Details DMS Final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\dms_msc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B46DC07-5545-4F0B-AAB9-E2F748B91E96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE13CB34-D65F-46DC-991C-502175DD8EE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>S.N</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Hall Short Name</t>
+  </si>
+  <si>
+    <t>RTH</t>
+  </si>
+  <si>
+    <t>Afrin Ahmed Eva</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>SHH</t>
   </si>
 </sst>
 </file>
@@ -401,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D8"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,14 +427,15 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -432,8 +448,11 @@
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -446,8 +465,11 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -460,8 +482,11 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -474,8 +499,11 @@
       <c r="D7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -487,6 +515,26 @@
       </c>
       <c r="D8" t="s">
         <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>41140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>